<commit_message>
Finalized Okofen data collection Periodic Script.
Changed sensor ID naming, started using a routine to identify changed
values to save reading space.
</commit_message>
<xml_diff>
--- a/bmsapp/scripts/files/New_Sensors.xlsx
+++ b/bmsapp/scripts/files/New_Sensors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="264">
   <si>
     <t>Site Outdoor Temp</t>
   </si>
@@ -732,167 +732,92 @@
     <t>id_val="chuvw_firing_rate_tot", slope=30000.0</t>
   </si>
   <si>
-    <t>hmr_StrHmT</t>
-  </si>
-  <si>
-    <t>hmr_GreenHsT</t>
-  </si>
-  <si>
-    <t>hmr_BoilerRmT</t>
-  </si>
-  <si>
-    <t>hmr_ArptTemp</t>
-  </si>
-  <si>
-    <t>hmr_ArptWind</t>
-  </si>
-  <si>
-    <t>hmr_OutdoorT</t>
-  </si>
-  <si>
-    <t>hmr_StrArrBtuMeter</t>
-  </si>
-  <si>
-    <t>hmr_StrArrInT</t>
-  </si>
-  <si>
-    <t>hmr_StrArrOutT</t>
-  </si>
-  <si>
-    <t>hmr_StrArrFlowMeter</t>
-  </si>
-  <si>
-    <t>hmr_GrnArrBtuMeter</t>
-  </si>
-  <si>
-    <t>hmr_GrnArrInT</t>
-  </si>
-  <si>
-    <t>hmr_GrnArrOutT</t>
-  </si>
-  <si>
-    <t>hmr_GrnArrFlowMeter</t>
-  </si>
-  <si>
-    <t>hmr_PoolT</t>
-  </si>
-  <si>
-    <t>hmr_PoolSoilT</t>
-  </si>
-  <si>
-    <t>hmr_PL750_bottom</t>
-  </si>
-  <si>
-    <t>hmr_PL750_mid</t>
-  </si>
-  <si>
-    <t>hmr_PL750_top</t>
-  </si>
-  <si>
-    <t>hmr_PriToPoolReturnT</t>
-  </si>
-  <si>
-    <t>hmr_PriLoopT</t>
-  </si>
-  <si>
-    <t>hmr_PoolToPriT</t>
-  </si>
-  <si>
-    <t>hmr_MixedT</t>
-  </si>
-  <si>
-    <t>hmr_BoilerStackT</t>
-  </si>
-  <si>
-    <t>Straw Home Temperature</t>
-  </si>
-  <si>
-    <t>Greenhouse Temperature</t>
-  </si>
-  <si>
-    <t>Homer Airport Temperature, F</t>
-  </si>
-  <si>
-    <t>Homer Airport Wind, mph</t>
-  </si>
-  <si>
-    <t>Site Outdoor Temperature, F</t>
-  </si>
-  <si>
-    <t>Straw Array Btu/hr</t>
-  </si>
-  <si>
-    <t>Straw Array Inlet Temp</t>
-  </si>
-  <si>
-    <t>Straw Array Outlet Temp</t>
-  </si>
-  <si>
-    <t>Straw Array Flow gpm</t>
-  </si>
-  <si>
-    <t>Greenhouse Array Btu/hr</t>
-  </si>
-  <si>
-    <t>Greenhouse Array Inlet Temp</t>
-  </si>
-  <si>
-    <t>Greenhouse Array Outlet Temp</t>
-  </si>
-  <si>
-    <t>Greenhouse Array Flow gpm</t>
-  </si>
-  <si>
-    <t>HS Tank Temp</t>
-  </si>
-  <si>
-    <t>Soil Temp Beside Tank</t>
-  </si>
-  <si>
-    <t>PL750 Tank Temp Bottom</t>
-  </si>
-  <si>
-    <t>PL750 Tank Temp Mid</t>
-  </si>
-  <si>
-    <t>PL750 Tank Temp Top</t>
-  </si>
-  <si>
-    <t>PL750 Heat Dump Temp</t>
-  </si>
-  <si>
-    <t>Primary Loop Temp</t>
-  </si>
-  <si>
-    <t>Strawbale Mixed Temp</t>
-  </si>
-  <si>
-    <t>Greenhouse Mixed Temp</t>
-  </si>
-  <si>
-    <t>Boiler Stack Temp</t>
-  </si>
-  <si>
-    <t>gpm</t>
-  </si>
-  <si>
-    <t>Homer Strawbale</t>
-  </si>
-  <si>
-    <t>Solar Thermal</t>
-  </si>
-  <si>
-    <t>Heat Storage</t>
-  </si>
-  <si>
-    <t>Heating System</t>
+    <t>Haines Senior Center</t>
+  </si>
+  <si>
+    <t>HainesSrCtr_boiler_1</t>
+  </si>
+  <si>
+    <t>Boiler Supply Temperature</t>
+  </si>
+  <si>
+    <t>Pellet Boiler</t>
+  </si>
+  <si>
+    <t>HainesSrCtr_P107</t>
+  </si>
+  <si>
+    <t>HainesSrCtr_P109</t>
+  </si>
+  <si>
+    <t>HainesSrCtr_P112</t>
+  </si>
+  <si>
+    <t>HainesSrCtr_P115</t>
+  </si>
+  <si>
+    <t>HainesSrCtr_P116</t>
+  </si>
+  <si>
+    <t>HainesSrCtr_P117</t>
+  </si>
+  <si>
+    <t>HainesSrCtr_P124</t>
+  </si>
+  <si>
+    <t>HainesSrCtr_P184</t>
+  </si>
+  <si>
+    <t>HainesSrCtr_P185</t>
+  </si>
+  <si>
+    <t>HainesSrCtr_P241</t>
+  </si>
+  <si>
+    <t>Flue/Flame Temperature, P107</t>
+  </si>
+  <si>
+    <t>Chip Temperature, P109</t>
+  </si>
+  <si>
+    <t>Burner Startups, P112</t>
+  </si>
+  <si>
+    <t>Boiler Off Time, P115</t>
+  </si>
+  <si>
+    <t>Auger Pulse, P116</t>
+  </si>
+  <si>
+    <t>Auger Pulse Off, P117</t>
+  </si>
+  <si>
+    <t>Flame Temperature Setpoint, P124</t>
+  </si>
+  <si>
+    <t>Speed AV, P184</t>
+  </si>
+  <si>
+    <t>A. Pulse / Vac On, P185</t>
+  </si>
+  <si>
+    <t>Boiler Status, P241</t>
+  </si>
+  <si>
+    <t>minutes</t>
+  </si>
+  <si>
+    <t>u / minute</t>
+  </si>
+  <si>
+    <t>count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -907,6 +832,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -938,7 +869,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -951,6 +882,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1572,17 +1506,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" customWidth="1"/>
     <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
@@ -1620,19 +1554,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>285</v>
+        <v>237</v>
       </c>
       <c r="B2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C2" t="s">
-        <v>261</v>
+        <v>239</v>
       </c>
       <c r="D2" t="s">
         <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>240</v>
       </c>
       <c r="F2">
         <v>10</v>
@@ -1640,19 +1574,19 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>285</v>
+        <v>237</v>
       </c>
       <c r="B3" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="C3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>240</v>
       </c>
       <c r="F3">
         <v>20</v>
@@ -1660,19 +1594,19 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>285</v>
+        <v>237</v>
       </c>
       <c r="B4" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>251</v>
       </c>
       <c r="D4" t="s">
         <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>240</v>
       </c>
       <c r="F4">
         <v>30</v>
@@ -1680,426 +1614,246 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>285</v>
+        <v>237</v>
       </c>
       <c r="B5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C5" t="s">
+        <v>252</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
         <v>240</v>
       </c>
-      <c r="C5" t="s">
-        <v>263</v>
-      </c>
-      <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1</v>
-      </c>
       <c r="F5">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>285</v>
+        <v>237</v>
       </c>
       <c r="B6" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C6" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>263</v>
       </c>
       <c r="E6" t="s">
-        <v>1</v>
+        <v>240</v>
       </c>
       <c r="F6">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>285</v>
+        <v>237</v>
       </c>
       <c r="B7" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C7" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>261</v>
       </c>
       <c r="E7" t="s">
-        <v>1</v>
+        <v>240</v>
       </c>
       <c r="F7">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>285</v>
+        <v>237</v>
       </c>
       <c r="B8" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C8" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="D8" t="s">
-        <v>164</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>286</v>
+        <v>240</v>
       </c>
       <c r="F8">
-        <v>10</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>285</v>
+        <v>237</v>
       </c>
       <c r="B9" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C9" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>286</v>
+        <v>240</v>
       </c>
       <c r="F9">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>285</v>
+        <v>237</v>
       </c>
       <c r="B10" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C10" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="D10" t="s">
         <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>286</v>
+        <v>240</v>
       </c>
       <c r="F10">
-        <v>30</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>285</v>
+        <v>237</v>
       </c>
       <c r="B11" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C11" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="D11" t="s">
-        <v>284</v>
+        <v>262</v>
       </c>
       <c r="E11" t="s">
-        <v>286</v>
+        <v>240</v>
       </c>
       <c r="F11">
-        <v>40</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>285</v>
+        <v>237</v>
       </c>
       <c r="B12" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C12" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="D12" t="s">
-        <v>164</v>
+        <v>220</v>
       </c>
       <c r="E12" t="s">
-        <v>286</v>
+        <v>240</v>
       </c>
       <c r="F12">
-        <v>50</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>285</v>
-      </c>
-      <c r="B13" t="s">
-        <v>248</v>
-      </c>
-      <c r="C13" t="s">
-        <v>271</v>
-      </c>
-      <c r="D13" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" t="s">
-        <v>286</v>
-      </c>
-      <c r="F13">
-        <v>60</v>
-      </c>
+      <c r="B13"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>285</v>
-      </c>
-      <c r="B14" t="s">
-        <v>249</v>
-      </c>
-      <c r="C14" t="s">
-        <v>272</v>
-      </c>
-      <c r="D14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" t="s">
-        <v>286</v>
-      </c>
-      <c r="F14">
-        <v>70</v>
-      </c>
+      <c r="B14"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>285</v>
-      </c>
-      <c r="B15" t="s">
-        <v>250</v>
-      </c>
-      <c r="C15" t="s">
-        <v>273</v>
-      </c>
-      <c r="D15" t="s">
-        <v>284</v>
-      </c>
-      <c r="E15" t="s">
-        <v>286</v>
-      </c>
-      <c r="F15">
-        <v>80</v>
-      </c>
+      <c r="B15"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>285</v>
-      </c>
-      <c r="B16" t="s">
-        <v>251</v>
-      </c>
-      <c r="C16" t="s">
-        <v>274</v>
-      </c>
-      <c r="D16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" t="s">
-        <v>287</v>
-      </c>
-      <c r="F16">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>285</v>
-      </c>
-      <c r="B17" t="s">
-        <v>252</v>
-      </c>
-      <c r="C17" t="s">
-        <v>275</v>
-      </c>
-      <c r="D17" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" t="s">
-        <v>287</v>
-      </c>
-      <c r="F17">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>285</v>
-      </c>
-      <c r="B18" t="s">
-        <v>253</v>
-      </c>
-      <c r="C18" t="s">
-        <v>276</v>
-      </c>
-      <c r="D18" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" t="s">
-        <v>287</v>
-      </c>
-      <c r="F18">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>285</v>
-      </c>
-      <c r="B19" t="s">
-        <v>254</v>
-      </c>
-      <c r="C19" t="s">
-        <v>277</v>
-      </c>
-      <c r="D19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" t="s">
-        <v>287</v>
-      </c>
-      <c r="F19">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>285</v>
-      </c>
-      <c r="B20" t="s">
-        <v>255</v>
-      </c>
-      <c r="C20" t="s">
-        <v>278</v>
-      </c>
-      <c r="D20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" t="s">
-        <v>287</v>
-      </c>
-      <c r="F20">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>285</v>
-      </c>
-      <c r="B21" t="s">
-        <v>256</v>
-      </c>
-      <c r="C21" t="s">
-        <v>279</v>
-      </c>
-      <c r="D21" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" t="s">
-        <v>287</v>
-      </c>
-      <c r="F21">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>285</v>
-      </c>
-      <c r="B22" t="s">
-        <v>257</v>
-      </c>
-      <c r="C22" t="s">
-        <v>280</v>
-      </c>
-      <c r="D22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" t="s">
-        <v>288</v>
-      </c>
-      <c r="F22">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>285</v>
-      </c>
-      <c r="B23" t="s">
-        <v>258</v>
-      </c>
-      <c r="C23" t="s">
-        <v>281</v>
-      </c>
-      <c r="D23" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" t="s">
-        <v>288</v>
-      </c>
-      <c r="F23">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>285</v>
-      </c>
-      <c r="B24" t="s">
-        <v>259</v>
-      </c>
-      <c r="C24" t="s">
-        <v>282</v>
-      </c>
-      <c r="D24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" t="s">
-        <v>288</v>
-      </c>
-      <c r="F24">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>285</v>
-      </c>
-      <c r="B25" t="s">
-        <v>260</v>
-      </c>
-      <c r="C25" t="s">
-        <v>283</v>
-      </c>
-      <c r="D25" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" t="s">
-        <v>288</v>
-      </c>
-      <c r="F25">
-        <v>40</v>
-      </c>
+      <c r="B16"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18"/>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30"/>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31"/>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>